<commit_message>
fix rtu01, 02-04 mengikuti
</commit_message>
<xml_diff>
--- a/IPC - Gateway - RTU Command Definition.xlsx
+++ b/IPC - Gateway - RTU Command Definition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Werk\gitProj\bigone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC96EB8F-B372-4B58-ACF2-FCA2271D3939}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAE870D-712F-4C37-AF8C-BA928C487FAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="3120" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="3030" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1614,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>